<commit_message>
initial regressions and functioned ones for fe but no treatment
</commit_message>
<xml_diff>
--- a/data/pcc_list_by_year.xlsx
+++ b/data/pcc_list_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukri-my.sharepoint.com/personal/james_currer_iuk_ukri_org/Documents/R/ecom185/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1610AAB-EEC7-4D7C-8212-C9B9725EE2EE}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E80A3F0-F9ED-4568-9446-A30D8E4ADB0B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34E50C65-FD83-4604-ABB6-390D6C2C0540}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17596" xr2:uid="{34E50C65-FD83-4604-ABB6-390D6C2C0540}"/>
   </bookViews>
   <sheets>
     <sheet name="changes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="94">
   <si>
     <t>Name in dataset</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Name in datawrapper</t>
   </si>
   <si>
-    <t>Changes?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Avon &amp; Somerset </t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>Metropolitan Police Service</t>
+  </si>
+  <si>
+    <t>Changes ex 2024</t>
   </si>
 </sst>
 </file>
@@ -1167,23 +1167,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F428D4-5E3C-43A7-B017-992D128723ED}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1328125" customWidth="1"/>
+    <col min="10" max="10" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1203,1135 +1203,1126 @@
         <v>2024</v>
       </c>
       <c r="G1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G42" si="0">IF(AND(C2=D2,D2=E2,E2=F2),"No change","Changes")</f>
+        <f>IF(AND(C2=D2,D2=E2),"No change","Changes")</f>
         <v>Changes</v>
       </c>
       <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(C3=D3,D3=E3),"No change","Changes")</f>
         <v>Changes</v>
       </c>
       <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
       </c>
       <c r="K3">
         <f>COUNTIF($G$2:$G$43,"="&amp;J3)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(AND(C4=D4,D4=E4),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+      <c r="J4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
       </c>
       <c r="K4">
         <f>COUNTIF($G$2:$G$43,"="&amp;J4)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="str">
+        <f>IF(AND(C5=D5,D5=E5),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IF(AND(C6=D6,D6=E6),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="str">
+        <f>IF(AND(C7=D7,D7=E7),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+      <c r="J7" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
       </c>
       <c r="K7">
         <f>COUNTIF($H$2:$H$43,"="&amp;J7)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(C8=D8,D8=E8),"No change","Changes")</f>
         <v>Changes</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8">
         <f>COUNTIF($H$2:$H$43,"="&amp;J8)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(C9=D9,D9=E9),"No change","Changes")</f>
         <v>No change</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9">
         <f>COUNTIF($H$2:$H$43,"="&amp;J9)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AND(C10=D10,D10=E10),"No change","Changes")</f>
         <v>Changes</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K10">
         <f>COUNTIF($H$2:$H$43,"="&amp;J10)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="str">
+        <f>IF(AND(C11=D11,D11=E11),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="str">
+        <f>IF(AND(C12=D12,D12=E12),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="str">
+        <f>IF(AND(C13=D13,D13=E13),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="str">
+        <f>IF(AND(C14=D14,D14=E14),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IF(AND(C15=D15,D15=E15),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="str">
+        <f>IF(AND(C16=D16,D16=E16),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="str">
+        <f>IF(AND(C17=D17,D17=E17),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="str">
+        <f>IF(AND(C18=D18,D18=E18),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="str">
+        <f>IF(AND(C19=D19,D19=E19),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="str">
+        <f>IF(AND(C20=D20,D20=E20),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="str">
+        <f>IF(AND(C21=D21,D21=E21),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="str">
+        <f>IF(AND(C22=D22,D22=E22),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="str">
+        <f>IF(AND(C23=D23,D23=E23),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="str">
+        <f>IF(AND(C24=D24,D24=E24),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" t="str">
+        <f>IF(AND(C25=D25,D25=E25),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="str">
+        <f>IF(AND(C26=D26,D26=E26),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="H26" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="str">
+        <f>IF(AND(C27=D27,D27=E27),"No change","Changes")</f>
         <v>No change</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" t="str">
+        <f>IF(AND(C28=D28,D28=E28),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" t="str">
+        <f>IF(AND(C29=D29,D29=E29),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" t="str">
+        <f>IF(AND(C30=D30,D30=E30),"No change","Changes")</f>
         <v>Changes</v>
       </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
+      <c r="H30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IF(AND(C31=D31,D31=E31),"No change","Changes")</f>
         <v>No change</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="str">
+        <f>IF(AND(C32=D32,D32=E32),"No change","Changes")</f>
         <v>No change</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" t="str">
+        <f>IF(AND(C33=D33,D33=E33),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="str">
+        <f>IF(AND(C34=D34,D34=E34),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" t="str">
+        <f>IF(AND(C35=D35,D35=E35),"No change","Changes")</f>
         <v>Changes</v>
       </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="0"/>
+      <c r="H35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" t="str">
+        <f>IF(AND(C36=D36,D36=E36),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="str">
+        <f>IF(AND(C37=D37,D37=E37),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" t="str">
+        <f>IF(AND(C38=D38,D38=E38),"No change","Changes")</f>
         <v>Changes</v>
       </c>
-      <c r="H16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
+      <c r="H38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" t="str">
+        <f>IF(AND(C39=D39,D39=E39),"No change","Changes")</f>
         <v>Changes</v>
       </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
+      <c r="H39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" t="str">
+        <f>IF(AND(C40=D40,D40=E40),"No change","Changes")</f>
         <v>No change</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" t="str">
+        <f>IF(AND(C41=D41,D41=E41),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" t="str">
+        <f>IF(AND(C42=D42,D42=E42),"No change","Changes")</f>
+        <v>No change</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" t="str">
+        <f>IF(AND(C43=D43,D43=E43),"No change","Changes")</f>
         <v>Changes</v>
       </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="0"/>
-        <v>Changes</v>
-      </c>
-      <c r="H39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" t="s">
-        <v>6</v>
-      </c>
-      <c r="G42" t="str">
-        <f t="shared" si="0"/>
-        <v>No change</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" t="str">
-        <f t="shared" ref="G43" si="1">IF(AND(C43=D43,D43=E43,E43=F43),"No change","Changes")</f>
-        <v>Changes</v>
-      </c>
       <c r="H43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2344,18 +2335,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A542E69-05A0-427A-BB88-A71DC7213BF2}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2408,12 +2399,12 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
         <f>B2</f>
@@ -2428,7 +2419,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="str">
         <f>F2</f>
@@ -2447,7 +2438,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" t="str">
         <f>K2</f>
@@ -2458,15 +2449,15 @@
         <v>Conservative</v>
       </c>
       <c r="N2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:E3" si="0">B3</f>
@@ -2481,7 +2472,7 @@
         <v>Labour</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:J3" si="1">F3</f>
@@ -2500,7 +2491,7 @@
         <v>Conservative</v>
       </c>
       <c r="K3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:M3" si="2">K3</f>
@@ -2511,15 +2502,15 @@
         <v>Conservative</v>
       </c>
       <c r="N3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:E4" si="3">B4</f>
@@ -2534,7 +2525,7 @@
         <v>Conservative</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" ref="G4:J4" si="4">F4</f>
@@ -2553,7 +2544,7 @@
         <v>Conservative</v>
       </c>
       <c r="K4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ref="L4:M4" si="5">K4</f>
@@ -2564,15 +2555,15 @@
         <v>Conservative</v>
       </c>
       <c r="N4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ref="C5:E5" si="6">B5</f>
@@ -2587,7 +2578,7 @@
         <v>Conservative</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:J5" si="7">F5</f>
@@ -2606,7 +2597,7 @@
         <v>Labour</v>
       </c>
       <c r="K5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:M5" si="8">K5</f>
@@ -2617,15 +2608,15 @@
         <v>Conservative</v>
       </c>
       <c r="N5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:E6" si="9">B6</f>
@@ -2640,7 +2631,7 @@
         <v>Labour</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" ref="G6:J6" si="10">F6</f>
@@ -2659,7 +2650,7 @@
         <v>Labour</v>
       </c>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ref="L6:M6" si="11">K6</f>
@@ -2670,15 +2661,15 @@
         <v>Conservative</v>
       </c>
       <c r="N6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:E7" si="12">B7</f>
@@ -2693,7 +2684,7 @@
         <v>Conservative</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7:J7" si="13">F7</f>
@@ -2712,7 +2703,7 @@
         <v>Conservative</v>
       </c>
       <c r="K7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ref="L7:M7" si="14">K7</f>
@@ -2723,15 +2714,15 @@
         <v>Conservative</v>
       </c>
       <c r="N7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" ref="C8:E8" si="15">B8</f>
@@ -2746,7 +2737,7 @@
         <v>Labour</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" ref="G8:J8" si="16">F8</f>
@@ -2765,7 +2756,7 @@
         <v>Labour</v>
       </c>
       <c r="K8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ref="L8:M8" si="17">K8</f>
@@ -2776,15 +2767,15 @@
         <v>Conservative</v>
       </c>
       <c r="N8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" ref="C9:E9" si="18">B9</f>
@@ -2799,7 +2790,7 @@
         <v>Conservative</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" ref="G9:J9" si="19">F9</f>
@@ -2818,7 +2809,7 @@
         <v>Conservative</v>
       </c>
       <c r="K9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ref="L9:M9" si="20">K9</f>
@@ -2829,15 +2820,15 @@
         <v>Conservative</v>
       </c>
       <c r="N9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ref="C10:E10" si="21">B10</f>
@@ -2852,7 +2843,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ref="G10:J10" si="22">F10</f>
@@ -2871,7 +2862,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="K10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ref="L10:M10" si="23">K10</f>
@@ -2882,15 +2873,15 @@
         <v>Conservative</v>
       </c>
       <c r="N10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:E11" si="24">B11</f>
@@ -2905,7 +2896,7 @@
         <v>Labour</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" ref="G11:J11" si="25">F11</f>
@@ -2924,7 +2915,7 @@
         <v>Labour</v>
       </c>
       <c r="K11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:M11" si="26">K11</f>
@@ -2935,15 +2926,15 @@
         <v>Labour</v>
       </c>
       <c r="N11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ref="C12:E12" si="27">B12</f>
@@ -2958,7 +2949,7 @@
         <v>Conservative</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" ref="G12:J12" si="28">F12</f>
@@ -2977,7 +2968,7 @@
         <v>Plaid Cymru</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ref="L12:M12" si="29">K12</f>
@@ -2988,15 +2979,15 @@
         <v>Plaid Cymru</v>
       </c>
       <c r="N12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ref="C13:E13" si="30">B13</f>
@@ -3011,7 +3002,7 @@
         <v>Conservative</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ref="G13:J13" si="31">F13</f>
@@ -3030,7 +3021,7 @@
         <v>Conservative</v>
       </c>
       <c r="K13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ref="L13:M13" si="32">K13</f>
@@ -3041,15 +3032,15 @@
         <v>Conservative</v>
       </c>
       <c r="N13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ref="C14:E14" si="33">B14</f>
@@ -3064,7 +3055,7 @@
         <v>Labour</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ref="G14:J14" si="34">F14</f>
@@ -3083,7 +3074,7 @@
         <v>Labour</v>
       </c>
       <c r="K14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ref="L14:M14" si="35">K14</f>
@@ -3094,15 +3085,15 @@
         <v>Labour</v>
       </c>
       <c r="N14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ref="C15:E15" si="36">B15</f>
@@ -3117,7 +3108,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ref="G15:J15" si="37">F15</f>
@@ -3136,7 +3127,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="K15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ref="L15:M15" si="38">K15</f>
@@ -3147,15 +3138,15 @@
         <v>Conservative</v>
       </c>
       <c r="N15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ref="C16:E16" si="39">B16</f>
@@ -3170,7 +3161,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ref="G16:J16" si="40">F16</f>
@@ -3189,7 +3180,7 @@
         <v>Labour</v>
       </c>
       <c r="K16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ref="L16:M16" si="41">K16</f>
@@ -3200,15 +3191,15 @@
         <v>Labour</v>
       </c>
       <c r="N16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ref="C17:E17" si="42">B17</f>
@@ -3223,7 +3214,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" ref="G17:J17" si="43">F17</f>
@@ -3242,7 +3233,7 @@
         <v>Conservative</v>
       </c>
       <c r="K17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ref="L17:M17" si="44">K17</f>
@@ -3253,15 +3244,15 @@
         <v>Conservative</v>
       </c>
       <c r="N17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ref="C18:E18" si="45">B18</f>
@@ -3276,7 +3267,7 @@
         <v>Conservative</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ref="G18:J18" si="46">F18</f>
@@ -3295,7 +3286,7 @@
         <v>Conservative</v>
       </c>
       <c r="K18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ref="L18:M18" si="47">K18</f>
@@ -3306,15 +3297,15 @@
         <v>Conservative</v>
       </c>
       <c r="N18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ref="C19:E19" si="48">B19</f>
@@ -3329,7 +3320,7 @@
         <v>Conservative</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ref="G19:J19" si="49">F19</f>
@@ -3348,7 +3339,7 @@
         <v>Labour</v>
       </c>
       <c r="K19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ref="L19:M19" si="50">K19</f>
@@ -3359,15 +3350,15 @@
         <v>Conservative</v>
       </c>
       <c r="N19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" ref="C20:E20" si="51">B20</f>
@@ -3382,7 +3373,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ref="G20:J20" si="52">F20</f>
@@ -3401,7 +3392,7 @@
         <v>Conservative</v>
       </c>
       <c r="K20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ref="L20:M20" si="53">K20</f>
@@ -3412,15 +3403,15 @@
         <v>Conservative</v>
       </c>
       <c r="N20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" ref="C21:E21" si="54">B21</f>
@@ -3435,7 +3426,7 @@
         <v>Labour</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21:J21" si="55">F21</f>
@@ -3454,7 +3445,7 @@
         <v>Labour</v>
       </c>
       <c r="K21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ref="L21:M21" si="56">K21</f>
@@ -3465,15 +3456,15 @@
         <v>Conservative</v>
       </c>
       <c r="N21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" ref="C22:E22" si="57">B22</f>
@@ -3488,7 +3479,7 @@
         <v>Conservative</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ref="G22:J22" si="58">F22</f>
@@ -3507,7 +3498,7 @@
         <v>Labour</v>
       </c>
       <c r="K22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ref="L22:M22" si="59">K22</f>
@@ -3518,15 +3509,15 @@
         <v>Conservative</v>
       </c>
       <c r="N22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" ref="C23:E23" si="60">B23</f>
@@ -3541,7 +3532,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ref="G23:J23" si="61">F23</f>
@@ -3560,7 +3551,7 @@
         <v>Conservative</v>
       </c>
       <c r="K23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ref="L23:M23" si="62">K23</f>
@@ -3571,15 +3562,15 @@
         <v>Conservative</v>
       </c>
       <c r="N23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" ref="C24:E24" si="63">B24</f>
@@ -3594,7 +3585,7 @@
         <v>Labour</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" ref="G24:J24" si="64">F24</f>
@@ -3613,7 +3604,7 @@
         <v>Labour</v>
       </c>
       <c r="K24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ref="L24:M24" si="65">K24</f>
@@ -3624,15 +3615,15 @@
         <v>Labour</v>
       </c>
       <c r="N24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" ref="C25:E25" si="66">B25</f>
@@ -3647,7 +3638,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25:J25" si="67">F25</f>
@@ -3666,7 +3657,7 @@
         <v>Conservative</v>
       </c>
       <c r="K25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ref="L25:M25" si="68">K25</f>
@@ -3677,15 +3668,15 @@
         <v>Conservative</v>
       </c>
       <c r="N25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" ref="C26:E26" si="69">B26</f>
@@ -3700,7 +3691,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ref="G26:J26" si="70">F26</f>
@@ -3719,7 +3710,7 @@
         <v>Plaid Cymru</v>
       </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ref="L26:M26" si="71">K26</f>
@@ -3730,15 +3721,15 @@
         <v>Labour</v>
       </c>
       <c r="N26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" ref="C27:E27" si="72">B27</f>
@@ -3753,7 +3744,7 @@
         <v>Conservative</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ref="G27:J27" si="73">F27</f>
@@ -3772,7 +3763,7 @@
         <v>Conservative</v>
       </c>
       <c r="K27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ref="L27:M27" si="74">K27</f>
@@ -3783,15 +3774,15 @@
         <v>Conservative</v>
       </c>
       <c r="N27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" ref="C28:E28" si="75">B28</f>
@@ -3806,7 +3797,7 @@
         <v>Conservative</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ref="G28:J28" si="76">F28</f>
@@ -3825,7 +3816,7 @@
         <v>Conservative</v>
       </c>
       <c r="K28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ref="L28:M28" si="77">K28</f>
@@ -3836,15 +3827,15 @@
         <v>Conservative</v>
       </c>
       <c r="N28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" ref="C29:E29" si="78">B29</f>
@@ -3859,7 +3850,7 @@
         <v>Labour</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" ref="G29:J29" si="79">F29</f>
@@ -3878,7 +3869,7 @@
         <v>Labour</v>
       </c>
       <c r="K29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ref="L29:M29" si="80">K29</f>
@@ -3889,15 +3880,15 @@
         <v>Labour</v>
       </c>
       <c r="N29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" ref="C30:E30" si="81">B30</f>
@@ -3912,7 +3903,7 @@
         <v>Labour</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" ref="G30:J30" si="82">F30</f>
@@ -3931,7 +3922,7 @@
         <v>Labour</v>
       </c>
       <c r="K30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ref="L30:M30" si="83">K30</f>
@@ -3942,15 +3933,15 @@
         <v>Conservative</v>
       </c>
       <c r="N30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" ref="C31:E31" si="84">B31</f>
@@ -3965,7 +3956,7 @@
         <v>Labour</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" ref="G31:J31" si="85">F31</f>
@@ -3984,7 +3975,7 @@
         <v>Labour</v>
       </c>
       <c r="K31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ref="L31:M31" si="86">K31</f>
@@ -3995,15 +3986,15 @@
         <v>Labour</v>
       </c>
       <c r="N31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" ref="C32:E32" si="87">B32</f>
@@ -4018,7 +4009,7 @@
         <v>Labour</v>
       </c>
       <c r="F32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" ref="G32:J32" si="88">F32</f>
@@ -4037,7 +4028,7 @@
         <v>Labour</v>
       </c>
       <c r="K32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" ref="L32:M32" si="89">K32</f>
@@ -4048,15 +4039,15 @@
         <v>Labour</v>
       </c>
       <c r="N32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" ref="C33:E33" si="90">B33</f>
@@ -4071,7 +4062,7 @@
         <v>Conservative</v>
       </c>
       <c r="F33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" ref="G33:J33" si="91">F33</f>
@@ -4090,7 +4081,7 @@
         <v>Conservative</v>
       </c>
       <c r="K33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" ref="L33:M33" si="92">K33</f>
@@ -4101,15 +4092,15 @@
         <v>Conservative</v>
       </c>
       <c r="N33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" ref="C34:E34" si="93">B34</f>
@@ -4124,7 +4115,7 @@
         <v>Conservative</v>
       </c>
       <c r="F34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" ref="G34:J34" si="94">F34</f>
@@ -4143,7 +4134,7 @@
         <v>Conservative</v>
       </c>
       <c r="K34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" ref="L34:M34" si="95">K34</f>
@@ -4154,15 +4145,15 @@
         <v>Conservative</v>
       </c>
       <c r="N34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" ref="C35:E35" si="96">B35</f>
@@ -4177,7 +4168,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" ref="G35:J35" si="97">F35</f>
@@ -4196,7 +4187,7 @@
         <v>Conservative</v>
       </c>
       <c r="K35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" ref="L35:M35" si="98">K35</f>
@@ -4207,15 +4198,15 @@
         <v>Conservative</v>
       </c>
       <c r="N35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" ref="C36:E36" si="99">B36</f>
@@ -4230,7 +4221,7 @@
         <v>Conservative</v>
       </c>
       <c r="F36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" ref="G36:J36" si="100">F36</f>
@@ -4249,7 +4240,7 @@
         <v>Conservative</v>
       </c>
       <c r="K36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" ref="L36:M36" si="101">K36</f>
@@ -4260,15 +4251,15 @@
         <v>Conservative</v>
       </c>
       <c r="N36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" ref="C37:E37" si="102">B37</f>
@@ -4283,7 +4274,7 @@
         <v>Conservative</v>
       </c>
       <c r="F37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" ref="G37:J37" si="103">F37</f>
@@ -4302,7 +4293,7 @@
         <v>Conservative</v>
       </c>
       <c r="K37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" ref="L37:M37" si="104">K37</f>
@@ -4313,15 +4304,15 @@
         <v>Conservative</v>
       </c>
       <c r="N37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" ref="C38:E38" si="105">B38</f>
@@ -4336,7 +4327,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" ref="G38:J38" si="106">F38</f>
@@ -4355,7 +4346,7 @@
         <v>Conservative</v>
       </c>
       <c r="K38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" ref="L38:M38" si="107">K38</f>
@@ -4366,15 +4357,15 @@
         <v>Conservative</v>
       </c>
       <c r="N38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" ref="C39:E39" si="108">B39</f>
@@ -4389,7 +4380,7 @@
         <v xml:space="preserve">Independent </v>
       </c>
       <c r="F39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" ref="G39:J39" si="109">F39</f>
@@ -4408,7 +4399,7 @@
         <v>Conservative</v>
       </c>
       <c r="K39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" ref="L39:M39" si="110">K39</f>
@@ -4419,15 +4410,15 @@
         <v>Conservative</v>
       </c>
       <c r="N39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" ref="C40:E40" si="111">B40</f>
@@ -4442,7 +4433,7 @@
         <v>Labour</v>
       </c>
       <c r="F40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ref="G40:J40" si="112">F40</f>
@@ -4461,7 +4452,7 @@
         <v>Labour</v>
       </c>
       <c r="K40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" ref="L40:M40" si="113">K40</f>
@@ -4472,15 +4463,15 @@
         <v>Labour</v>
       </c>
       <c r="N40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" ref="C41:E41" si="114">B41</f>
@@ -4495,7 +4486,7 @@
         <v>Labour</v>
       </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" ref="G41:J41" si="115">F41</f>
@@ -4514,7 +4505,7 @@
         <v>Labour</v>
       </c>
       <c r="K41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" ref="L41:M41" si="116">K41</f>
@@ -4525,15 +4516,15 @@
         <v>Labour</v>
       </c>
       <c r="N41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" ref="C42:E42" si="117">B42</f>
@@ -4548,7 +4539,7 @@
         <v>Conservative</v>
       </c>
       <c r="F42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" ref="G42:J42" si="118">F42</f>
@@ -4567,7 +4558,7 @@
         <v>Conservative</v>
       </c>
       <c r="K42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" ref="L42:M42" si="119">K42</f>
@@ -4578,15 +4569,15 @@
         <v>Conservative</v>
       </c>
       <c r="N42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" ref="C43:E43" si="120">B43</f>
@@ -4601,7 +4592,7 @@
         <v>Conservative</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" ref="G43:J43" si="121">F43</f>
@@ -4620,7 +4611,7 @@
         <v>Labour</v>
       </c>
       <c r="K43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" ref="L43:M43" si="122">K43</f>
@@ -4631,7 +4622,7 @@
         <v>Labour</v>
       </c>
       <c r="N43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
diff in diff starter script
</commit_message>
<xml_diff>
--- a/data/pcc_list_by_year.xlsx
+++ b/data/pcc_list_by_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukri-my.sharepoint.com/personal/james_currer_iuk_ukri_org/Documents/R/ecom185/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA537E37-0A33-4C61-8888-960E24E47083}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9D4F1D-BCB5-4B5C-ABB2-FFCAD842DD22}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="1440" windowWidth="24510" windowHeight="11910" xr2:uid="{34E50C65-FD83-4604-ABB6-390D6C2C0540}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="95">
   <si>
     <t>Name in dataset</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>Changes ex 2024</t>
+  </si>
+  <si>
+    <t>change type</t>
   </si>
 </sst>
 </file>
@@ -1165,11 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F428D4-5E3C-43A7-B017-992D128723ED}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,8 +1209,11 @@
       <c r="G1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1292,6 +1297,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1357,7 +1365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1380,6 +1388,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
       <c r="J7" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1445,6 +1456,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
       <c r="J9" t="s">
         <v>17</v>
       </c>
@@ -1453,7 +1467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1510,8 +1524,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1561,6 +1578,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1585,8 +1605,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1613,7 +1636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +1663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1667,7 +1690,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1690,8 +1713,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1718,7 +1744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1799,7 +1825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1849,8 +1875,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1877,7 +1906,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1904,7 +1933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1927,8 +1956,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1951,6 +1983,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1975,6 +2010,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2026,6 +2064,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2050,8 +2091,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2074,8 +2118,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -2098,8 +2145,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -2126,7 +2176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2149,8 +2199,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2173,8 +2226,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -2201,7 +2257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2251,6 +2307,9 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -2275,8 +2334,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -2299,8 +2361,11 @@
         <f t="shared" si="0"/>
         <v>No change</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -2328,13 +2393,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K43" xr:uid="{14F428D4-5E3C-43A7-B017-992D128723ED}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Labour"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K43" xr:uid="{14F428D4-5E3C-43A7-B017-992D128723ED}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated RDD and DiD
</commit_message>
<xml_diff>
--- a/data/pcc_list_by_year.xlsx
+++ b/data/pcc_list_by_year.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukri-my.sharepoint.com/personal/james_currer_iuk_ukri_org/Documents/R/ecom185/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9D4F1D-BCB5-4B5C-ABB2-FFCAD842DD22}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{EA12F45C-8752-4047-83DE-ECAE9BEEECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8B3BD2A-2661-49A9-BF91-C5C403086C93}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1440" windowWidth="24510" windowHeight="11910" xr2:uid="{34E50C65-FD83-4604-ABB6-390D6C2C0540}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{34E50C65-FD83-4604-ABB6-390D6C2C0540}"/>
   </bookViews>
   <sheets>
     <sheet name="changes" sheetId="1" r:id="rId1"/>
     <sheet name="wider" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">changes!$A$1:$K$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$G$43</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="95">
   <si>
     <t>Name in dataset</t>
   </si>
@@ -1170,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F428D4-5E3C-43A7-B017-992D128723ED}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,4 +4697,1125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFF55B6-F497-44A4-9DD7-5A45B6FB1284}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F43" si="0">IF(AND(C2=D2,D2=E2),"No change","Changes")</f>
+        <v>Changes</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <f>COUNTIF($F$2:$F$43,"="&amp;I3)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <f>COUNTIF($F$2:$F$43,"="&amp;I4)</f>
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <f>J4/SUM(J3:J4)</f>
+        <v>0.52380952380952384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF($G$2:$G$43,"="&amp;I7)</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K9" si="1">J7/SUM($J$7:$J$10)</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J10" si="2">COUNTIF($G$2:$G$43,"="&amp;I8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K10">
+        <f>J10/SUM($J$7:$J$10)</f>
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>No change</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>Changes</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G43" xr:uid="{8DFF55B6-F497-44A4-9DD7-5A45B6FB1284}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>